<commit_message>
all gems discovered up to x7
</commit_message>
<xml_diff>
--- a/Gems.xlsx
+++ b/Gems.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="20">
   <si>
     <t>Red</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Speed</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +769,9 @@
       <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -830,7 +835,9 @@
       <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
@@ -904,7 +911,9 @@
       <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -969,7 +978,9 @@
       <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="L8" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updated to work with new Bejeweled Blitz game
</commit_message>
<xml_diff>
--- a/Gems.xlsx
+++ b/Gems.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Pan\Desktop\Programs\C#\BejeweledBlitzEmperor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricPan-PC\Desktop\Programs\C# Projects\BejeweledBlitzEmperor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fail" sheetId="1" r:id="rId1"/>
     <sheet name="Retry" sheetId="2" r:id="rId2"/>
+    <sheet name="New" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="26">
   <si>
     <t>Red</t>
   </si>
@@ -85,6 +86,24 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>x10</t>
+  </si>
+  <si>
+    <t>Spinning</t>
+  </si>
+  <si>
+    <t>x11</t>
+  </si>
+  <si>
+    <t>x12</t>
   </si>
 </sst>
 </file>
@@ -696,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,4 +1007,361 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>